<commit_message>
fixing the bug - it was empty cells in the siltuximab parameter file
</commit_message>
<xml_diff>
--- a/parameters/ModelG_Siltuximab_Params_Kshama_7-22-19.xlsx
+++ b/parameters/ModelG_Siltuximab_Params_Kshama_7-22-19.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdoshi\Desktop\PK-PD Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/git/TMDD_EndogenousLigand/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5EFCBF-2068-4B2B-A39F-4C10508AB475}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D5D395-9CB7-6146-9EBA-139B68337460}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="11620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -108,6 +108,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -968,20 +969,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" zoomScale="92" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="92" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="26.625" customWidth="1"/>
-    <col min="6" max="6" width="10.875" customWidth="1"/>
-    <col min="9" max="9" width="24.125" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" customWidth="1"/>
     <col min="10" max="10" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1016,7 +1017,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1046,7 +1047,7 @@
       </c>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1076,7 +1077,7 @@
       </c>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1107,7 +1108,7 @@
       </c>
       <c r="J4" s="9"/>
     </row>
-    <row r="5" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1140,7 +1141,7 @@
       </c>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1171,7 +1172,7 @@
       </c>
       <c r="J6" s="9"/>
     </row>
-    <row r="7" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1202,7 +1203,7 @@
       </c>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1232,7 +1233,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1260,7 +1261,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1288,7 +1289,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1304,7 +1305,9 @@
       <c r="E11" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
       <c r="G11" s="5" t="s">
         <v>43</v>
       </c>
@@ -1316,7 +1319,7 @@
       </c>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1332,7 +1335,9 @@
       <c r="E12" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
       <c r="G12" s="5" t="s">
         <v>44</v>
       </c>
@@ -1344,7 +1349,7 @@
       </c>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1360,7 +1365,9 @@
       <c r="E13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
       <c r="G13" s="5" t="s">
         <v>7</v>
       </c>
@@ -1372,7 +1379,7 @@
       </c>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1388,7 +1395,9 @@
       <c r="E14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
       <c r="G14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1400,7 +1409,7 @@
       </c>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -1432,7 +1441,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -1464,7 +1473,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>17</v>
       </c>
@@ -1495,7 +1504,7 @@
       </c>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>18</v>
       </c>
@@ -1528,7 +1537,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>19</v>
       </c>
@@ -1560,7 +1569,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>20</v>
       </c>
@@ -1589,7 +1598,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>21</v>
       </c>
@@ -1621,7 +1630,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12">
         <v>22</v>
       </c>
@@ -1654,7 +1663,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
         <v>23</v>
       </c>
@@ -1688,7 +1697,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>24</v>
       </c>
@@ -1719,7 +1728,7 @@
       </c>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>25</v>
       </c>
@@ -1751,7 +1760,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>26</v>
       </c>
@@ -1781,7 +1790,7 @@
       </c>
       <c r="J26" s="9"/>
     </row>
-    <row r="27" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>27</v>
       </c>
@@ -1812,7 +1821,7 @@
       </c>
       <c r="J27" s="9"/>
     </row>
-    <row r="28" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>28</v>
       </c>
@@ -1844,7 +1853,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>29</v>
       </c>
@@ -1874,7 +1883,7 @@
       </c>
       <c r="J29" s="9"/>
     </row>
-    <row r="30" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>30</v>
       </c>
@@ -1905,7 +1914,7 @@
       </c>
       <c r="J30" s="9"/>
     </row>
-    <row r="31" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>31</v>
       </c>
@@ -1937,7 +1946,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>32</v>
       </c>
@@ -1969,7 +1978,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
         <v>33</v>
       </c>
@@ -1999,7 +2008,7 @@
       </c>
       <c r="J33" s="9"/>
     </row>
-    <row r="34" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8">
         <v>16</v>
       </c>
@@ -2031,10 +2040,10 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D39" s="3"/>
     </row>
   </sheetData>

</xml_diff>